<commit_message>
Australia Map Test Update
</commit_message>
<xml_diff>
--- a/artefacts/Test Cases - Australia Map.xlsx
+++ b/artefacts/Test Cases - Australia Map.xlsx
@@ -87,18 +87,6 @@
 </t>
   </si>
   <si>
-    <t>Test Case 1 Result: QUT International College</t>
-  </si>
-  <si>
-    <t>Test Case 3 Result: University of Queensland</t>
-  </si>
-  <si>
-    <t>Test Case 2 Result: State Library of Queensland</t>
-  </si>
-  <si>
-    <t>Test Case 4 Result: UQ/Mater McAuley Library</t>
-  </si>
-  <si>
     <t>Australia Map (User Story 17)</t>
   </si>
   <si>
@@ -157,6 +145,18 @@
   </si>
   <si>
     <t>TC_S17_04</t>
+  </si>
+  <si>
+    <t>Test Case 1 Result: Sydney</t>
+  </si>
+  <si>
+    <t>Test Case 4 Result: Canberra</t>
+  </si>
+  <si>
+    <t>Test Case 3 Result: Malbourne</t>
+  </si>
+  <si>
+    <t>Test Case 2 Result:  Adelaide</t>
   </si>
 </sst>
 </file>
@@ -323,22 +323,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>26404</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>97523</xdr:rowOff>
+      <xdr:colOff>14942</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>5835</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>29883</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
+      <xdr:colOff>155184</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19494</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEF59C5E-C7A0-481A-B138-D9B427A5C920}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7540468-54D6-46B8-881B-6E59E98EE05A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -360,8 +360,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7773404" y="10944817"/>
-          <a:ext cx="6248891" cy="3062536"/>
+          <a:off x="7761942" y="7087953"/>
+          <a:ext cx="6385654" cy="3420247"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -373,22 +373,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>24085</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>26713</xdr:rowOff>
+      <xdr:colOff>23001</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>30155</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>450321</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>82177</xdr:rowOff>
+      <xdr:colOff>163244</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>62549</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45B61DD-D148-4048-8F48-BF6A47EC929D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{563EA167-E5BE-4B80-AAC6-6451D015F452}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -410,8 +410,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7771085" y="7288125"/>
-          <a:ext cx="6671648" cy="3282758"/>
+          <a:off x="7770001" y="10698155"/>
+          <a:ext cx="6385655" cy="3438982"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -423,22 +423,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>29881</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>138721</xdr:rowOff>
+      <xdr:colOff>8647</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>29078</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>874248</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>44822</xdr:rowOff>
+      <xdr:colOff>1090184</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>10152</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C21DA576-145C-4359-A116-721E4BF1A6B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EB6A97E-E00A-4E8F-BD5D-9426D6C1BE03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -460,8 +460,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29881" y="7400133"/>
-          <a:ext cx="6148485" cy="3133395"/>
+          <a:off x="8647" y="10697078"/>
+          <a:ext cx="6385655" cy="3387662"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -473,22 +473,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7470</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>87253</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1127</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>838890</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>112060</xdr:rowOff>
+      <xdr:colOff>1081537</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>164353</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
+        <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59DC8E2A-7858-4485-A26F-47882631992F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD835B4B-E3D1-4DED-B6D9-3D907BC39ADF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -510,8 +510,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7470" y="10934547"/>
-          <a:ext cx="6135538" cy="3072807"/>
+          <a:off x="0" y="7083245"/>
+          <a:ext cx="6385655" cy="3390520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082C041C-A97C-4E4D-A10D-947B044BC46C}">
   <dimension ref="A2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,7 +851,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -914,20 +914,20 @@
     </row>
     <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="s">
@@ -936,20 +936,20 @@
     </row>
     <row r="12" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
@@ -958,20 +958,20 @@
     </row>
     <row r="13" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
@@ -980,20 +980,20 @@
     </row>
     <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
@@ -1032,18 +1032,18 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E39" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>